<commit_message>
Updated documentation, more of literature review written on shareLatex
</commit_message>
<xml_diff>
--- a/uartFFTadc/SupportFiles/MEMS/ExperimentalData.xlsx
+++ b/uartFFTadc/SupportFiles/MEMS/ExperimentalData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tim\Documents\GitHub\MScProject_EmbeddedSystems_ConditionMonitoring\uartFFTadc\SupportFiles\MEMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filestore.soton.ac.uk\users\tjg1g14\mydocuments\MScProject_EmbeddedSystems_ConditionMonitoring\uartFFTadc\SupportFiles\MEMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8784"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t>Periodic Test</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>ADXL354</t>
+  </si>
+  <si>
+    <t>Max(Converted)</t>
+  </si>
+  <si>
+    <t>RMS Acc</t>
   </si>
 </sst>
 </file>
@@ -106,6 +112,1051 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MMA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3053</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3095</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4053</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$5:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.36680000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35289999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.374</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36809999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3765</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.37430000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.38850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5413</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.61760000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5CEC-400E-A869-180B766B03D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>ADXL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3053</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3095</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4053</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$19:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.36680000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63680000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65590000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.81899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9944999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1779000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0070000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8922000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1960999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4377</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.49809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5CEC-400E-A869-180B766B03D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="979459872"/>
+        <c:axId val="979463200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="979459872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="979463200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="979463200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="979459872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,24 +1422,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M32"/>
+  <dimension ref="B2:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.3125" customWidth="1"/>
-    <col min="4" max="4" width="12.3125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -407,11 +1465,29 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
       <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -430,23 +1506,29 @@
       <c r="G5">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5">
+        <v>0.36680000000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R5">
+        <v>20</v>
+      </c>
+      <c r="S5">
+        <v>63</v>
+      </c>
+      <c r="T5">
+        <v>23</v>
+      </c>
+      <c r="U5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -465,23 +1547,29 @@
       <c r="G6">
         <v>6</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6">
+        <v>20</v>
+      </c>
+      <c r="S6">
+        <v>52</v>
+      </c>
+      <c r="T6">
+        <v>16</v>
+      </c>
+      <c r="U6">
         <v>7</v>
       </c>
-      <c r="J6">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>63</v>
-      </c>
-      <c r="L6">
-        <v>23</v>
-      </c>
-      <c r="M6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -500,23 +1588,14 @@
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7">
-        <v>20</v>
-      </c>
-      <c r="K7">
-        <v>52</v>
-      </c>
-      <c r="L7">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7">
+        <v>0.3785</v>
+      </c>
+      <c r="I7">
+        <v>0.22589999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -535,8 +1614,14 @@
       <c r="G8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8">
+        <v>0.36630000000000001</v>
+      </c>
+      <c r="I8">
+        <v>0.24249999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -555,8 +1640,14 @@
       <c r="G9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H9">
+        <v>0.374</v>
+      </c>
+      <c r="I9">
+        <v>0.21310000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -575,8 +1666,14 @@
       <c r="G10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H10">
+        <v>0.36809999999999998</v>
+      </c>
+      <c r="I10">
+        <v>0.24929999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -595,8 +1692,14 @@
       <c r="G11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H11">
+        <v>0.3765</v>
+      </c>
+      <c r="I11">
+        <v>0.18970000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -615,8 +1718,14 @@
       <c r="G12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12">
+        <v>0.37430000000000002</v>
+      </c>
+      <c r="I12">
+        <v>0.2581</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -635,8 +1744,14 @@
       <c r="G13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H13">
+        <v>0.38850000000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.18870000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -655,8 +1770,14 @@
       <c r="G14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14">
+        <v>0.4</v>
+      </c>
+      <c r="I14">
+        <v>0.27379999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -675,8 +1796,14 @@
       <c r="G15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="I15">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -695,8 +1822,14 @@
       <c r="G16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H16">
+        <v>0.42259999999999998</v>
+      </c>
+      <c r="I16">
+        <v>0.28939999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -715,8 +1848,14 @@
       <c r="G17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17">
+        <v>0.5413</v>
+      </c>
+      <c r="I17">
+        <v>0.29330000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -735,8 +1874,14 @@
       <c r="G18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H18">
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="I18">
+        <v>0.40579999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -755,8 +1900,14 @@
       <c r="G19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19">
+        <v>0.36680000000000001</v>
+      </c>
+      <c r="I19">
+        <v>0.2276</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -775,8 +1926,14 @@
       <c r="G20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I20">
+        <v>0.20949999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -795,8 +1952,14 @@
       <c r="G21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H21">
+        <v>0.63680000000000003</v>
+      </c>
+      <c r="I21">
+        <v>0.38869999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>9</v>
       </c>
@@ -815,8 +1978,14 @@
       <c r="G22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22">
+        <v>0.65590000000000004</v>
+      </c>
+      <c r="I22">
+        <v>0.41889999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -835,8 +2004,14 @@
       <c r="G23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H23">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="I23">
+        <v>0.43509999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>9</v>
       </c>
@@ -855,8 +2030,14 @@
       <c r="G24">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H24">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="I24">
+        <v>0.53979999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -875,8 +2056,14 @@
       <c r="G25">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H25">
+        <v>1.9944999999999999</v>
+      </c>
+      <c r="I25">
+        <v>1.1641999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>9</v>
       </c>
@@ -895,8 +2082,14 @@
       <c r="G26">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H26">
+        <v>2.1779000000000002</v>
+      </c>
+      <c r="I26">
+        <v>1.5025999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -915,8 +2108,14 @@
       <c r="G27">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27">
+        <v>3.0070000000000001</v>
+      </c>
+      <c r="I27">
+        <v>1.5125999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -935,8 +2134,14 @@
       <c r="G28">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H28">
+        <v>1.8922000000000001</v>
+      </c>
+      <c r="I28">
+        <v>1.3292999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -955,8 +2160,14 @@
       <c r="G29">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H29">
+        <v>2.1960999999999999</v>
+      </c>
+      <c r="I29">
+        <v>1.1238999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -975,8 +2186,14 @@
       <c r="G30">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H30">
+        <v>2.4377</v>
+      </c>
+      <c r="I30">
+        <v>1.6516</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -995,8 +2212,14 @@
       <c r="G31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H31">
+        <v>0.49809999999999999</v>
+      </c>
+      <c r="I31">
+        <v>0.27389999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -1015,8 +2238,15 @@
       <c r="G32">
         <v>4</v>
       </c>
+      <c r="H32">
+        <v>0.629</v>
+      </c>
+      <c r="I32">
+        <v>0.43509999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>